<commit_message>
21 / 7/ 2024
</commit_message>
<xml_diff>
--- a/05 Spiderman.xlsx
+++ b/05 Spiderman.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salvatore/Downloads/repofumetti/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF440A0B-BB1E-9A4E-86F1-F80813CB9964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676BBCB7-76F7-7E41-A263-5B766F7B26C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="36340" windowHeight="18800" activeTab="3" xr2:uid="{1338FCF8-35BB-4125-BC06-1B8E8F60BCCA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{1338FCF8-35BB-4125-BC06-1B8E8F60BCCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Riepilogo" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>Da</t>
   </si>
@@ -362,13 +362,22 @@
   </si>
   <si>
     <t>SEC da #1 a #379</t>
+  </si>
+  <si>
+    <t>Uomo Ragno Star Comics da #4 a #17 For Fans  Only #1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uomo Ragno Star Comics #27 a #29 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uomo Ragno Star Comics #33 a #35 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,6 +458,13 @@
       <color rgb="FF403F3F"/>
       <name val="Open Sans Condensed"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -477,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -496,6 +512,7 @@
     </xf>
     <xf numFmtId="17" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="17" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -876,10 +893,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DEA8871-6201-49B9-BDF4-88BE03D31DF7}">
-  <dimension ref="A4:D16"/>
+  <dimension ref="A4:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -951,6 +968,146 @@
       </c>
       <c r="D16" s="2" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18">
+        <v>221</v>
+      </c>
+      <c r="C18">
+        <v>230</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" s="14" customFormat="1">
+      <c r="B19" s="14">
+        <v>231</v>
+      </c>
+      <c r="C19" s="14">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20">
+        <v>237</v>
+      </c>
+      <c r="C20">
+        <v>241</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" s="14" customFormat="1">
+      <c r="B21" s="14">
+        <v>242</v>
+      </c>
+      <c r="C21" s="14">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22">
+        <v>246</v>
+      </c>
+      <c r="C22">
+        <v>248</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="14">
+        <v>249</v>
+      </c>
+      <c r="C23" s="14">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24">
+        <v>255</v>
+      </c>
+      <c r="C24">
+        <v>265</v>
+      </c>
+      <c r="D24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="14">
+        <v>266</v>
+      </c>
+      <c r="C25" s="14">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26">
+        <v>267</v>
+      </c>
+      <c r="C26">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="14">
+        <v>273</v>
+      </c>
+      <c r="C27" s="14">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28">
+        <v>293</v>
+      </c>
+      <c r="C28">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="14">
+        <v>295</v>
+      </c>
+      <c r="C29" s="14">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30">
+        <v>296</v>
+      </c>
+      <c r="C30">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="14">
+        <v>330</v>
+      </c>
+      <c r="C31" s="14">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32">
+        <v>364</v>
+      </c>
+      <c r="C32">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="14">
+        <v>371</v>
+      </c>
+      <c r="C33" s="14">
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -1056,7 +1213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B468F013-F939-44A4-B919-701DCFF3BB38}">
   <dimension ref="A4:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView topLeftCell="B32" zoomScale="309" zoomScaleNormal="309" workbookViewId="0">
       <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>

</xml_diff>